<commit_message>
UC1,2,3 DM, SSD, Usecase, TC fixed + UC1-AD
</commit_message>
<xml_diff>
--- a/Analysis/TC/FS-TC.xlsx
+++ b/Analysis/TC/FS-TC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="6120" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="6120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FS-UC1-seHistorik-TC" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>Nummer</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>login id : cpr?</t>
+  </si>
+  <si>
+    <t>ekstra passagerer : de øvrige op til 4 for 50% rabat (antal af passagerer max 5)</t>
   </si>
 </sst>
 </file>
@@ -589,8 +592,8 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1089,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1103,7 +1106,9 @@
         <v>40</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -1459,7 +1464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
seHistorik + pris calculation : prototype
</commit_message>
<xml_diff>
--- a/Analysis/TC/FS-TC.xlsx
+++ b/Analysis/TC/FS-TC.xlsx
@@ -142,24 +142,12 @@
     <t>1) Jesper, 01-05-2016, 31-05-2016, Herning, 45,5 kr., Antal passagerer : 4, Antal ture : 2                        2) Juyoung, 01-05-2016, 31-05-2016, Herning, 28 kr., Antal passagerer : 3, Antal ture : 1</t>
   </si>
   <si>
-    <t>pris : 17,5 kr.</t>
-  </si>
-  <si>
     <t>Der er manglende obligatoriske oplysninger i kundens input</t>
   </si>
   <si>
-    <t>pris : 28 kr.</t>
-  </si>
-  <si>
     <t>pris : 35 kr.</t>
   </si>
   <si>
-    <t>Dato : 20-06-2016, Fra Kommune : Herning, Til Kommune : Aarhus, Antal Passagerer : 3, Ekstra tilbehør : 0, kommentar : ""</t>
-  </si>
-  <si>
-    <t>Dato : 21-06-2016, Fra Kommune : Herning, Til Kommune : Aarhus, Antal Passagerer : 1,  Ekstra tilbehør : kørestole, kommentar : ""</t>
-  </si>
-  <si>
     <t>Dato : 20-06-2016, Fra Kommune : Herning, Antal Passagerer : 1</t>
   </si>
   <si>
@@ -218,6 +206,18 @@
   </si>
   <si>
     <t>ekstra passagerer : de øvrige op til 4 for 50% rabat (antal af passagerer max 5)</t>
+  </si>
+  <si>
+    <t>Dato : 20-06-2016, Fra Kommune : Herning, Til Kommune : Aarhus, Antal Passagerer : 3, Ekstra tilbehør : 0, kommentar : "" afstand : 100km</t>
+  </si>
+  <si>
+    <t>pris : 2800 kr.</t>
+  </si>
+  <si>
+    <t>Dato : 21-06-2016, Fra Kommune : Herning, Til Kommune : Herning, Antal Passagerer : 1,  Ekstra tilbehør : kørestole, kommentar : "" afstand : 10km</t>
+  </si>
+  <si>
+    <t>pris : 140 kr.</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,14 +1100,14 @@
         <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -1119,10 +1119,10 @@
         <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1133,13 +1133,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1150,13 +1150,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1167,13 +1167,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1513,17 +1513,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -1532,13 +1532,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1549,13 +1549,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1566,13 +1566,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>

</xml_diff>

<commit_message>
UC6 Usecase, AD, SSD
</commit_message>
<xml_diff>
--- a/Analysis/TC/FS-TC.xlsx
+++ b/Analysis/TC/FS-TC.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
   <si>
     <t>Nummer</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>setFraDato(null)</t>
-  </si>
-  <si>
-    <t>det skal ikke komme til FSController - rolleback : UC1_HistorikSøgning</t>
   </si>
   <si>
     <t>UC1_OC2.java</t>
@@ -565,8 +562,8 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>40</v>
@@ -649,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>40</v>
@@ -672,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>40</v>
@@ -695,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>40</v>
@@ -718,13 +715,13 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -739,9 +736,6 @@
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>40</v>
@@ -752,16 +746,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">

</xml_diff>

<commit_message>
all exported af pdf
</commit_message>
<xml_diff>
--- a/Analysis/TC/FS-TC.xlsx
+++ b/Analysis/TC/FS-TC.xlsx
@@ -580,7 +580,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD4"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,22 +716,22 @@
       <c r="A9" s="6">
         <v>4</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -739,22 +739,22 @@
       <c r="A10" s="6">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -762,7 +762,7 @@
       <c r="A11" s="6">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -774,7 +774,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1011,7 +1012,7 @@
     <mergeCell ref="B1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1020,7 +1021,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1409,7 +1410,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>